<commit_message>
feat: all but companies
</commit_message>
<xml_diff>
--- a/economic_game_ministers_with_passwords.xlsx
+++ b/economic_game_ministers_with_passwords.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,40 +436,35 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>lastname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>lastname</t>
+          <t>firstname</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>firstname</t>
+          <t>middlename</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>middlename</t>
+          <t>email</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>email</t>
+          <t>cash</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cash</t>
+          <t>password</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>password</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>sent</t>
         </is>
@@ -479,78 +474,72 @@
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Балабанов</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Балабан</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Балабанович</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>itsagaydak@edu.hse.ru</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>500</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>mjoSk</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
         <v>0</v>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Балабанов</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>Балабан</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Балабанович</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>itsagaydak@edu.hse.ru</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>500</v>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>mjoSk</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="n">
-        <v>1</v>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Балаболов</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Балаболов</t>
+          <t>Балабол</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Балабол</t>
+          <t>Балаболович</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Балаболович</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>m.s.v.inkognito@gmail.com</t>
         </is>
       </c>
-      <c r="G3" t="n">
+      <c r="F3" t="n">
         <v>1000</v>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>HiPpM</t>
         </is>
       </c>
-      <c r="I3" t="n">
-        <v>1</v>
+      <c r="H3" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>